<commit_message>
Hardware V1.1 schematic and firmware test updated
</commit_message>
<xml_diff>
--- a/Datasheets/Resistor range calcs.xlsx
+++ b/Datasheets/Resistor range calcs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewgeppert/Dropbox/Electronics/SAO_Etch_sAo_Sketch/Datasheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F3D6EE-5FC1-6445-8D62-47B783FB55E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD866B4F-34C0-B54C-8729-8D1E3E734F6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1300" yWindow="8660" windowWidth="22840" windowHeight="17440" xr2:uid="{CEEAB7D7-F79D-9D47-9894-C0841CF73BB4}"/>
+    <workbookView xWindow="3440" yWindow="9880" windowWidth="22840" windowHeight="17440" xr2:uid="{CEEAB7D7-F79D-9D47-9894-C0841CF73BB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
   <si>
     <t>R2</t>
   </si>
@@ -50,22 +50,28 @@
     <t>Target V</t>
   </si>
   <si>
-    <t>RV_POT_5K</t>
-  </si>
-  <si>
     <t>Calc'd</t>
   </si>
   <si>
     <t>Test Results</t>
+  </si>
+  <si>
+    <t>ADC Calc Range to Use</t>
+  </si>
+  <si>
+    <t>ADC Test Counts</t>
+  </si>
+  <si>
+    <t>Pico W 3.3V Reg Output</t>
+  </si>
+  <si>
+    <t>RV_POT_5K in parallel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.000"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -75,12 +81,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -95,9 +107,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,82 +446,163 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B0C9075-7356-9045-A8E2-CFC5AD1A4F7D}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="2"/>
+      <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2">
         <v>3.3</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>10000</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C4">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2">
         <v>1.6</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="3">
         <f>3.3*((B7+B5)/(B3+B5+B7))</f>
-        <v>1.6248730964467004</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>5000</v>
-      </c>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C6">
+        <v>1.3813953488372093</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1.39</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2">
+        <v>-4000</v>
+      </c>
+      <c r="I4" s="2">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2500</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2">
         <v>0.8</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="3">
         <f>C2*((B7)/(B3+B5+B7))</f>
-        <v>0.78730964467005071</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+        <v>0.90174418604651152</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.89</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2">
+        <v>32512</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>4700</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C8">
+      <c r="C7" s="2"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>2</v>
       </c>
@@ -515,18 +610,18 @@
         <v>3</v>
       </c>
       <c r="D11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" t="s">
         <v>5</v>
       </c>
-      <c r="E11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C12">
         <v>3.3</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -534,37 +629,31 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C14">
         <v>1.6</v>
       </c>
       <c r="D14" s="1">
         <f>3.3*((B17+B15)/(B13+B15+B17))</f>
-        <v>1.6333333333333333</v>
-      </c>
-      <c r="E14">
-        <v>1.42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1.392485549132948</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B15">
-        <v>5000</v>
+        <v>2500</v>
       </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C16">
         <v>0.8</v>
       </c>
       <c r="D16" s="1">
         <f>C12*((B17)/(B13+B15+B17))</f>
-        <v>0.79999999999999993</v>
-      </c>
-      <c r="E16">
-        <v>0.9</v>
+        <v>0.91560693641618485</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -588,10 +677,10 @@
         <v>3</v>
       </c>
       <c r="D21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" t="s">
         <v>5</v>
-      </c>
-      <c r="E21" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -613,18 +702,15 @@
       </c>
       <c r="D24" s="1">
         <f>3.3*((B27+B25)/(B23+B25+B27))</f>
-        <v>1.7966666666666664</v>
-      </c>
-      <c r="E24">
-        <v>1.42</v>
+        <v>1.5541935483870966</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B25">
-        <v>5000</v>
+        <v>2500</v>
       </c>
       <c r="D25" s="1"/>
     </row>
@@ -634,10 +720,7 @@
       </c>
       <c r="D26" s="1">
         <f>C22*((B27)/(B23+B25+B27))</f>
-        <v>0.87999999999999989</v>
-      </c>
-      <c r="E26">
-        <v>0.9</v>
+        <v>1.0219354838709678</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>